<commit_message>
added readme and add street header
</commit_message>
<xml_diff>
--- a/Data_rev.xlsx
+++ b/Data_rev.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CAMH137222\OneDrive - WSP O365\Documents\testhere\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A46B589-DE1F-4245-9141-7013C4E73080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EAEC2FB-0B08-41A6-A5BC-8CD989224AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="67">
   <si>
     <t>Bikes</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>Site Code 2</t>
+  </si>
+  <si>
+    <t>Street name</t>
   </si>
 </sst>
 </file>
@@ -1832,7 +1835,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{407B395F-BA9A-4859-B080-DE5ADEF772AC}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1847,6 +1852,9 @@
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>65</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
       </c>
       <c r="C1" t="s">
         <v>42</v>
@@ -2130,6 +2138,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B1A0D63259FBA848B34211FF238C275D" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bb9d81aab52b024b73d5c6386321c0b5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="323ad87a-8af6-4c6c-a04d-46183120dd34" xmlns:ns3="0dbb9613-057a-4ae2-a1fa-9a89c406c5e8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bdb2e7cfe41a5371f80e16bdff3171ae" ns2:_="" ns3:_="">
     <xsd:import namespace="323ad87a-8af6-4c6c-a04d-46183120dd34"/>
@@ -2346,15 +2363,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19927E65-B844-4722-92CF-5961BAAD8465}">
   <ds:schemaRefs>
@@ -2367,6 +2375,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48AD7FF7-4573-4920-8EE8-32B9778A774D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBDBFE4F-A204-4C35-ACEE-A6B65CA9A1EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2385,14 +2401,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48AD7FF7-4573-4920-8EE8-32B9778A774D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{59096ad9-8b60-446a-90b7-017dbb9421a3}" enabled="1" method="Standard" siteId="{3d234255-e20f-4205-88a5-9658a402999b}" contentBits="0" removed="0"/>

</xml_diff>